<commit_message>
Added test cases to com.verizon
</commit_message>
<xml_diff>
--- a/com.verizon/src/test/resources/TestData.xlsx
+++ b/com.verizon/src/test/resources/TestData.xlsx
@@ -1,32 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\com.att\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5692E4AA-85B2-41D5-B273-4FC0E57C238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="11" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
-    <sheet name="Expedia" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
-    <sheet name="ATT" sheetId="4" r:id="rId4"/>
-    <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
-    <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId9"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId10"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId11"/>
-    <sheet name="Chase" sheetId="12" r:id="rId12"/>
-    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId14"/>
+    <sheet name="TopLeftMenu" sheetId="15" r:id="rId1"/>
+    <sheet name="TopCenterMenu" sheetId="17" r:id="rId2"/>
+    <sheet name="TopHamburgerMenu" sheetId="18" r:id="rId3"/>
+    <sheet name="PhoneMenuBar" sheetId="19" r:id="rId4"/>
+    <sheet name="Brands" sheetId="20" r:id="rId5"/>
+    <sheet name="DeviceCondition" sheetId="21" r:id="rId6"/>
+    <sheet name="OS" sheetId="22" r:id="rId7"/>
+    <sheet name="Featured" sheetId="23" r:id="rId8"/>
+    <sheet name="Prices" sheetId="24" r:id="rId9"/>
+    <sheet name="Colors" sheetId="25" r:id="rId10"/>
+    <sheet name="SortBy" sheetId="26" r:id="rId11"/>
+    <sheet name="Counts" sheetId="27" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,19 +45,264 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Center Menu</t>
+  </si>
+  <si>
+    <t>Explore wireless</t>
+  </si>
+  <si>
+    <t>Plans &amp; prices</t>
+  </si>
+  <si>
+    <t>Phones &amp; devices</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Bring your own</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Wireless deals</t>
+  </si>
+  <si>
+    <t>Left Menu</t>
+  </si>
+  <si>
+    <t>Deals &amp; discounts</t>
+  </si>
+  <si>
+    <t>Home phone</t>
+  </si>
+  <si>
+    <t>Bundles</t>
+  </si>
+  <si>
+    <t>Smart technology</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Find a store</t>
+  </si>
+  <si>
+    <t>Check order status</t>
+  </si>
+  <si>
+    <t>My favorites</t>
+  </si>
+  <si>
+    <t>Hamburger Menu</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>AT&amp;T PREPAID</t>
+  </si>
+  <si>
+    <t>Tablets &amp; Laptops</t>
+  </si>
+  <si>
+    <t>Smartwatches</t>
+  </si>
+  <si>
+    <t>Hotspots &amp; more</t>
+  </si>
+  <si>
+    <t>Phone Menu Bar</t>
+  </si>
+  <si>
+    <t>Brands</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>AT&amp;T</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Kyocera</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Motorola</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>Sonim</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Apple iOS</t>
+  </si>
+  <si>
+    <t>Featured</t>
+  </si>
+  <si>
+    <t>5G capable</t>
+  </si>
+  <si>
+    <t>Low cost</t>
+  </si>
+  <si>
+    <t>Wi-Fi calling</t>
+  </si>
+  <si>
+    <t>Foldables</t>
+  </si>
+  <si>
+    <t>Prices</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>$10 or less</t>
+  </si>
+  <si>
+    <t>$10 - $25</t>
+  </si>
+  <si>
+    <t>$25 - $50</t>
+  </si>
+  <si>
+    <t>$50 - $100</t>
+  </si>
+  <si>
+    <t>$100 or more</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Sort By</t>
+  </si>
+  <si>
+    <t>Best-selling</t>
+  </si>
+  <si>
+    <t>Price: low to high</t>
+  </si>
+  <si>
+    <t>Price: high to low</t>
+  </si>
+  <si>
+    <t>Newest</t>
+  </si>
+  <si>
+    <t>Rating: high to low</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,8 +328,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,142 +645,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E464D8A-6350-4BC5-B9EB-BA5543395498}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030D8EA2-D510-423A-8DBC-B0C663F9BB44}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA0E140-B35A-4736-B2BE-46B36ACA85DF}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CF7C2B-BE69-4FEE-8D2B-ED1505E50A5F}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4ED8F-84C7-4351-B184-022F160E827E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB124C4-9CEE-457F-95C0-47C63DA908AF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA0B8EC-E04F-491E-87C2-487F73A9BC0A}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -543,52 +919,356 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59BB938-FA52-426E-9DD7-96F933A4DBB1}">
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CA77FC-C852-40C4-B844-304E3F0A9E58}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BE9415-B459-437D-BFF9-3AE3B6C86EF1}">
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3918AE-9AED-408E-A737-2CD333BC5256}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EF3C9A-44FD-4C22-BD17-61B3536591C3}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1812F7-1E54-4333-9F5C-99ABD4AA8E3D}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC34C28-8436-4011-B5AF-40480AF98457}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>